<commit_message>
For real this time
</commit_message>
<xml_diff>
--- a/Documents/Rule_List.xlsx
+++ b/Documents/Rule_List.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="45">
   <si>
     <t xml:space="preserve">SCRUM NUMBER</t>
   </si>
@@ -98,40 +98,6 @@
   </si>
   <si>
     <t xml:space="preserve">http://docs.aws.amazon.com/storagegateway/latest/APIReference/API_AddUploadBuffer.html</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">¯\_(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Microsoft YaHei"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">ツ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">)_/¯ </t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">http://loli.dance/</t>
   </si>
   <si>
     <t xml:space="preserve">Instance Sharing Code</t>
@@ -198,7 +164,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -309,12 +275,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Microsoft YaHei"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="9">
@@ -577,7 +537,7 @@
   <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G17" activeCellId="0" sqref="G17"/>
+      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -773,22 +733,16 @@
       <c r="C17" s="0" t="n">
         <v>16</v>
       </c>
-      <c r="E17" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="G17" s="0" t="s">
-        <v>27</v>
-      </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C18" s="0" t="n">
         <v>17</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -796,7 +750,7 @@
         <v>18</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -804,7 +758,7 @@
         <v>19</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -812,10 +766,10 @@
         <v>20</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -823,10 +777,10 @@
         <v>21</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -834,10 +788,10 @@
         <v>22</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -845,10 +799,10 @@
         <v>23</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -856,10 +810,10 @@
         <v>24</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -867,10 +821,10 @@
         <v>25</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -878,10 +832,10 @@
         <v>26</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -889,10 +843,10 @@
         <v>27</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -900,10 +854,10 @@
         <v>28</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>